<commit_message>
Updated code as of 02July2020
</commit_message>
<xml_diff>
--- a/data/MultipleTestData.xlsx
+++ b/data/MultipleTestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MultipleUsers" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="MultipleGroup" sheetId="5" r:id="rId3"/>
     <sheet name="ParentLevelTestData" sheetId="3" r:id="rId4"/>
     <sheet name="SubLevelTestData" sheetId="4" r:id="rId5"/>
+    <sheet name="paralleltest" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="200">
   <si>
     <t>Username</t>
   </si>
@@ -62,42 +64,27 @@
     <t>QMS/EC/00</t>
   </si>
   <si>
-    <t>QMS Engineering Change</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
     <t>QMS/WI/00</t>
   </si>
   <si>
-    <t>QMS WorkInstructions</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>QMS/QM/00</t>
   </si>
   <si>
-    <t>QMS Quality Manual</t>
-  </si>
-  <si>
     <t>QMS/P/00</t>
   </si>
   <si>
-    <t>QMS Procedures</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
     <t>QMS/CL/00</t>
   </si>
   <si>
-    <t>QMS CheckLists</t>
-  </si>
-  <si>
     <t>reviewDue</t>
   </si>
   <si>
@@ -110,10 +97,6 @@
     <t>QMS/CL/QCL/0</t>
   </si>
   <si>
-    <t xml:space="preserve">QMS CheckLists
-</t>
-  </si>
-  <si>
     <t>subLevelName</t>
   </si>
   <si>
@@ -279,21 +262,6 @@
     <t>(NA)</t>
   </si>
   <si>
-    <t>01.QMSCL</t>
-  </si>
-  <si>
-    <t>01.QA</t>
-  </si>
-  <si>
-    <t>01.Management Manual</t>
-  </si>
-  <si>
-    <t>WI &amp; TC</t>
-  </si>
-  <si>
-    <t>Change request @ CR152</t>
-  </si>
-  <si>
     <t>QMS/P/QA/</t>
   </si>
   <si>
@@ -456,9 +424,6 @@
     <t>WI &amp; TC(R2)</t>
   </si>
   <si>
-    <t>Change request @ CR152(R3)</t>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
@@ -474,18 +439,6 @@
     <t>37</t>
   </si>
   <si>
-    <t>295-4(VHR1)</t>
-  </si>
-  <si>
-    <t>295-5(VHR1)</t>
-  </si>
-  <si>
-    <t>295-6(VHR2)</t>
-  </si>
-  <si>
-    <t>295-7(VHR2)</t>
-  </si>
-  <si>
     <t>routeName</t>
   </si>
   <si>
@@ -495,68 +448,185 @@
     <t>minNumofApproversReqd</t>
   </si>
   <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>1st round non mandatory  2nd Round with All Approvers Reqd</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>2 rounds with some mandatory and some non mandatory and mentioned mim number of approvers reqd</t>
+  </si>
+  <si>
+    <t>All Approvers Reqd(1 round,2 approvers)</t>
+  </si>
+  <si>
+    <t>(VH</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>Doc Pro Position based Approver</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>2 Approvers in a position</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>1 round having 2 approvers and another round has position based approvers</t>
+  </si>
+  <si>
     <t>(VH1)</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>1st round non mandatory  2nd Round with All Approvers Reqd</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>2 rounds with some mandatory and some non mandatory and mentioned mim number of approvers reqd</t>
-  </si>
-  <si>
-    <t>All Approvers Reqd(1 round,2 approvers)</t>
-  </si>
-  <si>
-    <t>(VH</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>position</t>
-  </si>
-  <si>
-    <t>Doc Pro Position based Approver</t>
-  </si>
-  <si>
-    <t>desc</t>
-  </si>
-  <si>
-    <t>2 Approvers in a position</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>1 round having 2 approvers and another round has position based approvers</t>
+    <t>295-4(VH1)</t>
+  </si>
+  <si>
+    <t>295-5(VH1)</t>
+  </si>
+  <si>
+    <t>295-7(VH)</t>
+  </si>
+  <si>
+    <t>295-6(VH)</t>
+  </si>
+  <si>
+    <t>ECR @ CR152(R3)</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>01.Quality Manual(R1)</t>
+  </si>
+  <si>
+    <t>02.Quality Policy(AbA)</t>
+  </si>
+  <si>
+    <t>QMS/P-:</t>
+  </si>
+  <si>
+    <t>03.Finance Department(PbR)</t>
+  </si>
+  <si>
+    <t>QMS/FD</t>
+  </si>
+  <si>
+    <t>04. Human Resources(R2)</t>
+  </si>
+  <si>
+    <t>QMS-HM-</t>
+  </si>
+  <si>
+    <t>05.Operations(R3)</t>
+  </si>
+  <si>
+    <t>QMS/OP@</t>
+  </si>
+  <si>
+    <t>3 . A Develop &amp; Monitor Annual Budget</t>
+  </si>
+  <si>
+    <t>4.i Core Data Procedures</t>
+  </si>
+  <si>
+    <t>2.1Quality Objectives</t>
+  </si>
+  <si>
+    <t>QMS/P-QO:-</t>
+  </si>
+  <si>
+    <t>QMS/FD*D&amp;A-</t>
+  </si>
+  <si>
+    <t>QMS-HM-(4.i)CDP#</t>
+  </si>
+  <si>
+    <t>5a.Consolidation/Closing of Facilities</t>
+  </si>
+  <si>
+    <t>QMS/OP@C/C:</t>
+  </si>
+  <si>
+    <t>3.A.i Transfer Requests</t>
+  </si>
+  <si>
+    <t>QMS/FD*TR-</t>
+  </si>
+  <si>
+    <t>4i.iEmployee Requisitions</t>
+  </si>
+  <si>
+    <t>QMS-HM-(4i.i)CDP#ER-</t>
+  </si>
+  <si>
+    <t>4i.iiW/C Off Work Status</t>
+  </si>
+  <si>
+    <t>QMS-HM-(4i.ii)CDP#W/C-</t>
+  </si>
+  <si>
+    <t>5b.Re-Draw Attendance Boundaries Work Instructions</t>
+  </si>
+  <si>
+    <t>QMS/OP@RE:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,7 +643,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -586,8 +656,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -610,12 +686,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -626,12 +713,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -693,7 +791,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -725,10 +823,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -760,7 +857,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -936,16 +1032,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="S45" sqref="S45"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
@@ -968,15 +1064,15 @@
     <col min="23" max="23" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -1000,48 +1096,48 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="T1" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -1050,24 +1146,24 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K2" s="2"/>
@@ -1079,14 +1175,14 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="9"/>
+      <c r="T2" s="8"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23">
       <c r="A3" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -1095,24 +1191,24 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="2"/>
@@ -1124,12 +1220,12 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-      <c r="T3" s="9"/>
+      <c r="T3" s="8"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1140,24 +1236,24 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="2"/>
@@ -1169,14 +1265,14 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
-      <c r="T4" s="9"/>
+      <c r="T4" s="8"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23">
       <c r="A5" s="4" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
@@ -1185,19 +1281,19 @@
         <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>2</v>
@@ -1214,14 +1310,14 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
-      <c r="T5" s="9"/>
+      <c r="T5" s="8"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23">
       <c r="A6" s="4" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -1230,24 +1326,24 @@
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K6" s="2"/>
@@ -1259,14 +1355,14 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
-      <c r="T6" s="9"/>
+      <c r="T6" s="8"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23">
       <c r="A7" s="4" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>10</v>
@@ -1275,24 +1371,24 @@
         <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K7" s="2"/>
@@ -1304,14 +1400,14 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
-      <c r="T7" s="9"/>
+      <c r="T7" s="8"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23">
       <c r="A8" s="4" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -1320,24 +1416,24 @@
         <v>11</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K8" s="2"/>
@@ -1349,14 +1445,14 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
-      <c r="T8" s="9"/>
+      <c r="T8" s="8"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23">
       <c r="A9" s="4" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
@@ -1365,24 +1461,24 @@
         <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K9" s="2"/>
@@ -1394,14 +1490,14 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
-      <c r="T9" s="9"/>
+      <c r="T9" s="8"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23">
       <c r="A10" s="4" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -1410,24 +1506,24 @@
         <v>11</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K10" s="2"/>
@@ -1439,14 +1535,14 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-      <c r="T10" s="9"/>
+      <c r="T10" s="8"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
@@ -1455,24 +1551,24 @@
         <v>11</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K11" s="2"/>
@@ -1484,14 +1580,14 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
-      <c r="T11" s="9"/>
+      <c r="T11" s="8"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23">
       <c r="A12" s="4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>10</v>
@@ -1500,24 +1596,24 @@
         <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K12" s="2"/>
@@ -1529,19 +1625,19 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
-      <c r="T12" s="9"/>
+      <c r="T12" s="8"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23">
       <c r="A13" s="4" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="2"/>
@@ -1560,19 +1656,19 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
-      <c r="T13" s="9"/>
+      <c r="T13" s="8"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23">
       <c r="A14" s="4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="4"/>
@@ -1591,19 +1687,19 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
-      <c r="T14" s="9"/>
+      <c r="T14" s="8"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="14.25" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="4"/>
@@ -1622,174 +1718,174 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
-      <c r="T15" s="9"/>
+      <c r="T15" s="8"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="16" spans="1:23" s="12" customFormat="1">
+      <c r="A16" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="1:23" s="12" customFormat="1">
+      <c r="A17" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+    </row>
+    <row r="18" spans="1:23" s="12" customFormat="1">
+      <c r="A18" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+    </row>
+    <row r="19" spans="1:23" s="12" customFormat="1">
+      <c r="A19" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+    </row>
+    <row r="20" spans="1:23" s="12" customFormat="1">
+      <c r="A20" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="4"/>
@@ -1808,19 +1904,19 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
-      <c r="T21" s="9"/>
+      <c r="T21" s="8"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23">
       <c r="A22" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="4"/>
@@ -1839,19 +1935,19 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
-      <c r="T22" s="9"/>
+      <c r="T22" s="8"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23">
       <c r="A23" s="4" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="4"/>
@@ -1870,14 +1966,14 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
-      <c r="T23" s="9"/>
+      <c r="T23" s="8"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23">
       <c r="A24" s="4" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>10</v>
@@ -1893,13 +1989,13 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1907,14 +2003,14 @@
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
-      <c r="T24" s="9"/>
+      <c r="T24" s="8"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23">
       <c r="A25" s="4" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>10</v>
@@ -1930,10 +2026,10 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>12</v>
@@ -1944,14 +2040,14 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
-      <c r="T25" s="9"/>
+      <c r="T25" s="8"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23">
       <c r="A26" s="4" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>10</v>
@@ -1967,13 +2063,13 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -1981,14 +2077,14 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
-      <c r="T26" s="9"/>
+      <c r="T26" s="8"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23">
       <c r="A27" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>10</v>
@@ -2004,13 +2100,13 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -2018,14 +2114,14 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
-      <c r="T27" s="9"/>
+      <c r="T27" s="8"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23">
       <c r="A28" s="4" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>10</v>
@@ -2041,7 +2137,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>13</v>
@@ -2055,14 +2151,14 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
-      <c r="T28" s="9"/>
+      <c r="T28" s="8"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23">
       <c r="A29" s="4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>10</v>
@@ -2078,32 +2174,32 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="Q29" s="4" t="s">
         <v>12</v>
       </c>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
-      <c r="T29" s="9"/>
+      <c r="T29" s="8"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23">
       <c r="A30" s="4" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>10</v>
@@ -2119,32 +2215,32 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
-      <c r="T30" s="9"/>
+      <c r="T30" s="8"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23">
       <c r="A31" s="4" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>10</v>
@@ -2160,32 +2256,32 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="Q31" s="4" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
-      <c r="T31" s="9"/>
+      <c r="T31" s="8"/>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23">
       <c r="A32" s="4" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>10</v>
@@ -2201,32 +2297,32 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
-      <c r="T32" s="9"/>
+      <c r="T32" s="8"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23">
       <c r="A33" s="4" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>10</v>
@@ -2242,41 +2338,41 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
-      <c r="T33" s="9"/>
+      <c r="T33" s="8"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23">
       <c r="A34" s="4" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -2292,26 +2388,26 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="S34" s="2"/>
-      <c r="T34" s="9"/>
+      <c r="T34" s="8"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23">
       <c r="A35" s="4" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -2327,61 +2423,61 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="S35" s="2"/>
-      <c r="T35" s="9"/>
+      <c r="T35" s="8"/>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:23" s="12" customFormat="1">
+      <c r="A36" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="S36" s="2"/>
-      <c r="T36" s="9"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="S36" s="10"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
+      <c r="W36" s="10"/>
+    </row>
+    <row r="37" spans="1:23">
       <c r="A37" s="4" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -2397,26 +2493,26 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="S37" s="2"/>
-      <c r="T37" s="9"/>
+      <c r="T37" s="8"/>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23">
       <c r="A38" s="4" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -2432,17 +2528,17 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="S38" s="2"/>
-      <c r="T38" s="9"/>
+      <c r="T38" s="8"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
       <c r="W38" s="2"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23">
       <c r="A39" s="4" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>10</v>
@@ -2451,7 +2547,7 @@
         <v>11</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -2468,64 +2564,64 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
-      <c r="T39" s="9"/>
+      <c r="T39" s="8"/>
       <c r="U39" s="2"/>
       <c r="V39" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="W39" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="T40" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
-      <c r="W40" s="2"/>
-    </row>
-    <row r="41" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="W39" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" s="12" customFormat="1">
+      <c r="A40" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="T40" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="10"/>
+    </row>
+    <row r="41" spans="1:23" ht="30">
       <c r="A41" s="4" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -2542,27 +2638,27 @@
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
       <c r="S41" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="T41" s="9" t="s">
-        <v>161</v>
+        <v>143</v>
+      </c>
+      <c r="T41" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
       <c r="W41" s="2"/>
     </row>
-    <row r="42" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" ht="45">
       <c r="A42" s="4" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -2579,29 +2675,29 @@
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
       <c r="S42" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="T42" s="9" t="s">
-        <v>163</v>
+        <v>145</v>
+      </c>
+      <c r="T42" s="8" t="s">
+        <v>146</v>
       </c>
       <c r="U42" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
     </row>
-    <row r="43" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" ht="30">
       <c r="A43" s="4" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -2618,16 +2714,313 @@
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
       <c r="S43" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="T43" s="9" t="s">
-        <v>176</v>
+        <v>158</v>
+      </c>
+      <c r="T43" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="U43" s="2"/>
       <c r="V43" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="W43" s="2"/>
+    </row>
+    <row r="44" spans="1:23">
+      <c r="A44" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+    </row>
+    <row r="45" spans="1:23">
+      <c r="A45" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="8"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+    </row>
+    <row r="46" spans="1:23">
+      <c r="A46" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+    </row>
+    <row r="47" spans="1:23">
+      <c r="A47" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="8"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+    </row>
+    <row r="48" spans="1:23">
+      <c r="A48" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="8"/>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48" s="2"/>
+    </row>
+    <row r="49" spans="1:23">
+      <c r="A49" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="W43" s="2"/>
+      <c r="B49" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="8"/>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
+    </row>
+    <row r="50" spans="1:23">
+      <c r="A50" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="8"/>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
+    </row>
+    <row r="51" spans="1:23">
+      <c r="A51" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="8"/>
+      <c r="U51" s="2"/>
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+    </row>
+    <row r="52" spans="1:23">
+      <c r="A52" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="2"/>
+      <c r="V52" s="2"/>
+      <c r="W52" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2648,29 +3041,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -2694,9 +3087,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -2705,19 +3098,19 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
@@ -2726,9 +3119,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -2737,19 +3130,19 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>2</v>
@@ -2758,12 +3151,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -2776,12 +3169,12 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2</v>
@@ -2804,14 +3197,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -2820,7 +3213,7 @@
     <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2831,78 +3224,78 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2911,27 +3304,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2939,101 +3328,97 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="C6" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3043,14 +3428,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" customWidth="1"/>
@@ -3060,7 +3445,7 @@
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3068,143 +3453,340 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="C2" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="G11" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="E15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>